<commit_message>
add new version for the query
</commit_message>
<xml_diff>
--- a/code/static/aapl.xlsx
+++ b/code/static/aapl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\09060.gary.wu\code\FlaskRESTfulAPI\code\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCA3500-09E8-4F51-9364-53FBFCED5AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C5DE88-8522-4280-9B6E-08825A5012BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="480" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2028" yWindow="3228" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1 - Input Data" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Personal Required Rate of Return</t>
   </si>
   <si>
-    <t>6.86%</t>
+    <t>6.87%</t>
   </si>
   <si>
     <t>Shares Outstanding (M)</t>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H10" s="14">
         <f>G10*(1+B16)/(B15-B16)</f>
-        <v>1457975.1371205566</v>
+        <v>1454981.3483379679</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="H14" s="14">
         <f>H10/H13</f>
-        <v>1121519.336246582</v>
+        <v>1119216.4217984369</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B15" s="29" t="str">
         <f>'Step1 - Input Data'!B4</f>
-        <v>6.86%</v>
+        <v>6.87%</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="B17" s="14">
         <f>SUM(D14:H14)</f>
-        <v>1337211.2929994669</v>
+        <v>1334908.378551322</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B19" s="32">
         <f>B17/B18</f>
-        <v>308.82477898371059</v>
+        <v>308.29292807189887</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>